<commit_message>
tests pass with new implementation
</commit_message>
<xml_diff>
--- a/tests/testthat/_snaps/knitxl/data.frame1.xlsx
+++ b/tests/testthat/_snaps/knitxl/data.frame1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t xml:space="preserve">Volvo 142E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## Error in xl_obj$insert_data_frame(df, style = style, h_style = h_style, : object 'cropping_df' not found</t>
   </si>
 </sst>
 </file>
@@ -151,13 +154,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -180,8 +189,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1729,6 +1739,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
refactor with sew to implement code chunks
</commit_message>
<xml_diff>
--- a/tests/testthat/_snaps/knitxl/data.frame1.xlsx
+++ b/tests/testthat/_snaps/knitxl/data.frame1.xlsx
@@ -14,6 +14,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
+    <t xml:space="preserve">mtcars</t>
+  </si>
+  <si>
     <t xml:space="preserve"/>
   </si>
   <si>
@@ -144,9 +147,6 @@
   </si>
   <si>
     <t xml:space="preserve">Volvo 142E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">## Error in xl_obj$insert_data_frame(df, style = style, h_style = h_style, : object 'cropping_df' not found</t>
   </si>
 </sst>
 </file>
@@ -164,9 +164,8 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <b/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
     </font>
   </fonts>
   <fills count="2">
@@ -486,146 +485,75 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="n">
-        <v>21</v>
-      </c>
-      <c r="C2" t="n">
-        <v>6</v>
-      </c>
-      <c r="D2" t="n">
-        <v>160</v>
-      </c>
-      <c r="E2" t="n">
-        <v>110</v>
-      </c>
-      <c r="F2" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2.62</v>
-      </c>
-      <c r="H2" t="n">
-        <v>16.46</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>4</v>
-      </c>
-      <c r="L2" t="n">
-        <v>4</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="n">
-        <v>21</v>
-      </c>
-      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="n">
-        <v>160</v>
-      </c>
-      <c r="E3" t="n">
-        <v>110</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2.875</v>
-      </c>
-      <c r="H3" t="n">
-        <v>17.02</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>4</v>
-      </c>
-      <c r="L3" t="n">
-        <v>4</v>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="n">
-        <v>22.8</v>
+        <v>21</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="E4" t="n">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="F4" t="n">
-        <v>3.85</v>
+        <v>3.9</v>
       </c>
       <c r="G4" t="n">
-        <v>2.32</v>
+        <v>2.62</v>
       </c>
       <c r="H4" t="n">
-        <v>18.61</v>
+        <v>16.46</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
         <v>1</v>
@@ -634,109 +562,109 @@
         <v>4</v>
       </c>
       <c r="L4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="n">
-        <v>21.4</v>
+        <v>21</v>
       </c>
       <c r="C5" t="n">
         <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>258</v>
+        <v>160</v>
       </c>
       <c r="E5" t="n">
         <v>110</v>
       </c>
       <c r="F5" t="n">
-        <v>3.08</v>
+        <v>3.9</v>
       </c>
       <c r="G5" t="n">
-        <v>3.215</v>
+        <v>2.875</v>
       </c>
       <c r="H5" t="n">
-        <v>19.44</v>
+        <v>17.02</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="n">
-        <v>18.7</v>
+        <v>22.8</v>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>360</v>
+        <v>108</v>
       </c>
       <c r="E6" t="n">
-        <v>175</v>
+        <v>93</v>
       </c>
       <c r="F6" t="n">
-        <v>3.15</v>
+        <v>3.85</v>
       </c>
       <c r="G6" t="n">
-        <v>3.44</v>
+        <v>2.32</v>
       </c>
       <c r="H6" t="n">
-        <v>17.02</v>
+        <v>18.61</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="n">
-        <v>18.1</v>
+        <v>21.4</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>225</v>
+        <v>258</v>
       </c>
       <c r="E7" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F7" t="n">
-        <v>2.76</v>
+        <v>3.08</v>
       </c>
       <c r="G7" t="n">
-        <v>3.46</v>
+        <v>3.215</v>
       </c>
       <c r="H7" t="n">
-        <v>20.22</v>
+        <v>19.44</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
@@ -753,10 +681,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>14.3</v>
+        <v>18.7</v>
       </c>
       <c r="C8" t="n">
         <v>8</v>
@@ -765,16 +693,16 @@
         <v>360</v>
       </c>
       <c r="E8" t="n">
-        <v>245</v>
+        <v>175</v>
       </c>
       <c r="F8" t="n">
-        <v>3.21</v>
+        <v>3.15</v>
       </c>
       <c r="G8" t="n">
-        <v>3.57</v>
+        <v>3.44</v>
       </c>
       <c r="H8" t="n">
-        <v>15.84</v>
+        <v>17.02</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -786,33 +714,33 @@
         <v>3</v>
       </c>
       <c r="L8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="n">
-        <v>24.4</v>
+        <v>18.1</v>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D9" t="n">
-        <v>146.7</v>
+        <v>225</v>
       </c>
       <c r="E9" t="n">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="F9" t="n">
-        <v>3.69</v>
+        <v>2.76</v>
       </c>
       <c r="G9" t="n">
-        <v>3.19</v>
+        <v>3.46</v>
       </c>
       <c r="H9" t="n">
-        <v>20</v>
+        <v>20.22</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
@@ -821,74 +749,74 @@
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="n">
-        <v>22.8</v>
+        <v>14.3</v>
       </c>
       <c r="C10" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D10" t="n">
-        <v>140.8</v>
+        <v>360</v>
       </c>
       <c r="E10" t="n">
-        <v>95</v>
+        <v>245</v>
       </c>
       <c r="F10" t="n">
-        <v>3.92</v>
+        <v>3.21</v>
       </c>
       <c r="G10" t="n">
-        <v>3.15</v>
+        <v>3.57</v>
       </c>
       <c r="H10" t="n">
-        <v>22.9</v>
+        <v>15.84</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="n">
-        <v>19.2</v>
+        <v>24.4</v>
       </c>
       <c r="C11" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>167.6</v>
+        <v>146.7</v>
       </c>
       <c r="E11" t="n">
-        <v>123</v>
+        <v>62</v>
       </c>
       <c r="F11" t="n">
-        <v>3.92</v>
+        <v>3.69</v>
       </c>
       <c r="G11" t="n">
-        <v>3.44</v>
+        <v>3.19</v>
       </c>
       <c r="H11" t="n">
-        <v>18.3</v>
+        <v>20</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
@@ -900,33 +828,33 @@
         <v>4</v>
       </c>
       <c r="L11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="n">
-        <v>17.8</v>
+        <v>22.8</v>
       </c>
       <c r="C12" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D12" t="n">
-        <v>167.6</v>
+        <v>140.8</v>
       </c>
       <c r="E12" t="n">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="F12" t="n">
         <v>3.92</v>
       </c>
       <c r="G12" t="n">
-        <v>3.44</v>
+        <v>3.15</v>
       </c>
       <c r="H12" t="n">
-        <v>18.9</v>
+        <v>22.9</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
@@ -938,91 +866,91 @@
         <v>4</v>
       </c>
       <c r="L12" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="n">
-        <v>16.4</v>
+        <v>19.2</v>
       </c>
       <c r="C13" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D13" t="n">
-        <v>275.8</v>
+        <v>167.6</v>
       </c>
       <c r="E13" t="n">
-        <v>180</v>
+        <v>123</v>
       </c>
       <c r="F13" t="n">
-        <v>3.07</v>
+        <v>3.92</v>
       </c>
       <c r="G13" t="n">
-        <v>4.07</v>
+        <v>3.44</v>
       </c>
       <c r="H13" t="n">
-        <v>17.4</v>
+        <v>18.3</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="n">
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" t="n">
-        <v>17.3</v>
+        <v>17.8</v>
       </c>
       <c r="C14" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14" t="n">
-        <v>275.8</v>
+        <v>167.6</v>
       </c>
       <c r="E14" t="n">
-        <v>180</v>
+        <v>123</v>
       </c>
       <c r="F14" t="n">
-        <v>3.07</v>
+        <v>3.92</v>
       </c>
       <c r="G14" t="n">
-        <v>3.73</v>
+        <v>3.44</v>
       </c>
       <c r="H14" t="n">
-        <v>17.6</v>
+        <v>18.9</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="n">
-        <v>15.2</v>
+        <v>16.4</v>
       </c>
       <c r="C15" t="n">
         <v>8</v>
@@ -1037,10 +965,10 @@
         <v>3.07</v>
       </c>
       <c r="G15" t="n">
-        <v>3.78</v>
+        <v>4.07</v>
       </c>
       <c r="H15" t="n">
-        <v>18</v>
+        <v>17.4</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1057,28 +985,28 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="n">
-        <v>10.4</v>
+        <v>17.3</v>
       </c>
       <c r="C16" t="n">
         <v>8</v>
       </c>
       <c r="D16" t="n">
-        <v>472</v>
+        <v>275.8</v>
       </c>
       <c r="E16" t="n">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="F16" t="n">
-        <v>2.93</v>
+        <v>3.07</v>
       </c>
       <c r="G16" t="n">
-        <v>5.25</v>
+        <v>3.73</v>
       </c>
       <c r="H16" t="n">
-        <v>17.98</v>
+        <v>17.6</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -1090,33 +1018,33 @@
         <v>3</v>
       </c>
       <c r="L16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="n">
-        <v>10.4</v>
+        <v>15.2</v>
       </c>
       <c r="C17" t="n">
         <v>8</v>
       </c>
       <c r="D17" t="n">
-        <v>460</v>
+        <v>275.8</v>
       </c>
       <c r="E17" t="n">
-        <v>215</v>
+        <v>180</v>
       </c>
       <c r="F17" t="n">
-        <v>3</v>
+        <v>3.07</v>
       </c>
       <c r="G17" t="n">
-        <v>5.424</v>
+        <v>3.78</v>
       </c>
       <c r="H17" t="n">
-        <v>17.82</v>
+        <v>18</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1128,33 +1056,33 @@
         <v>3</v>
       </c>
       <c r="L17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" t="n">
-        <v>14.7</v>
+        <v>10.4</v>
       </c>
       <c r="C18" t="n">
         <v>8</v>
       </c>
       <c r="D18" t="n">
-        <v>440</v>
+        <v>472</v>
       </c>
       <c r="E18" t="n">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="F18" t="n">
-        <v>3.23</v>
+        <v>2.93</v>
       </c>
       <c r="G18" t="n">
-        <v>5.345</v>
+        <v>5.25</v>
       </c>
       <c r="H18" t="n">
-        <v>17.42</v>
+        <v>17.98</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1171,104 +1099,104 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" t="n">
-        <v>32.4</v>
+        <v>10.4</v>
       </c>
       <c r="C19" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D19" t="n">
-        <v>78.7</v>
+        <v>460</v>
       </c>
       <c r="E19" t="n">
-        <v>66</v>
+        <v>215</v>
       </c>
       <c r="F19" t="n">
-        <v>4.08</v>
+        <v>3</v>
       </c>
       <c r="G19" t="n">
-        <v>2.2</v>
+        <v>5.424</v>
       </c>
       <c r="H19" t="n">
-        <v>19.47</v>
+        <v>17.82</v>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L19" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="n">
-        <v>30.4</v>
+        <v>14.7</v>
       </c>
       <c r="C20" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D20" t="n">
-        <v>75.7</v>
+        <v>440</v>
       </c>
       <c r="E20" t="n">
-        <v>52</v>
+        <v>230</v>
       </c>
       <c r="F20" t="n">
-        <v>4.93</v>
+        <v>3.23</v>
       </c>
       <c r="G20" t="n">
-        <v>1.615</v>
+        <v>5.345</v>
       </c>
       <c r="H20" t="n">
-        <v>18.52</v>
+        <v>17.42</v>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L20" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" t="n">
-        <v>33.9</v>
+        <v>32.4</v>
       </c>
       <c r="C21" t="n">
         <v>4</v>
       </c>
       <c r="D21" t="n">
-        <v>71.1</v>
+        <v>78.7</v>
       </c>
       <c r="E21" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F21" t="n">
-        <v>4.22</v>
+        <v>4.08</v>
       </c>
       <c r="G21" t="n">
-        <v>1.835</v>
+        <v>2.2</v>
       </c>
       <c r="H21" t="n">
-        <v>19.9</v>
+        <v>19.47</v>
       </c>
       <c r="I21" t="n">
         <v>1</v>
@@ -1285,107 +1213,107 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" t="n">
-        <v>21.5</v>
+        <v>30.4</v>
       </c>
       <c r="C22" t="n">
         <v>4</v>
       </c>
       <c r="D22" t="n">
-        <v>120.1</v>
+        <v>75.7</v>
       </c>
       <c r="E22" t="n">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="F22" t="n">
-        <v>3.7</v>
+        <v>4.93</v>
       </c>
       <c r="G22" t="n">
-        <v>2.465</v>
+        <v>1.615</v>
       </c>
       <c r="H22" t="n">
-        <v>20.01</v>
+        <v>18.52</v>
       </c>
       <c r="I22" t="n">
         <v>1</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" t="n">
-        <v>15.5</v>
+        <v>33.9</v>
       </c>
       <c r="C23" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D23" t="n">
-        <v>318</v>
+        <v>71.1</v>
       </c>
       <c r="E23" t="n">
-        <v>150</v>
+        <v>65</v>
       </c>
       <c r="F23" t="n">
-        <v>2.76</v>
+        <v>4.22</v>
       </c>
       <c r="G23" t="n">
-        <v>3.52</v>
+        <v>1.835</v>
       </c>
       <c r="H23" t="n">
-        <v>16.87</v>
+        <v>19.9</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" t="n">
-        <v>15.2</v>
+        <v>21.5</v>
       </c>
       <c r="C24" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D24" t="n">
-        <v>304</v>
+        <v>120.1</v>
       </c>
       <c r="E24" t="n">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="F24" t="n">
-        <v>3.15</v>
+        <v>3.7</v>
       </c>
       <c r="G24" t="n">
-        <v>3.435</v>
+        <v>2.465</v>
       </c>
       <c r="H24" t="n">
-        <v>17.3</v>
+        <v>20.01</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="n">
         <v>0</v>
@@ -1394,33 +1322,33 @@
         <v>3</v>
       </c>
       <c r="L24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" t="n">
-        <v>13.3</v>
+        <v>15.5</v>
       </c>
       <c r="C25" t="n">
         <v>8</v>
       </c>
       <c r="D25" t="n">
-        <v>350</v>
+        <v>318</v>
       </c>
       <c r="E25" t="n">
-        <v>245</v>
+        <v>150</v>
       </c>
       <c r="F25" t="n">
-        <v>3.73</v>
+        <v>2.76</v>
       </c>
       <c r="G25" t="n">
-        <v>3.84</v>
+        <v>3.52</v>
       </c>
       <c r="H25" t="n">
-        <v>15.41</v>
+        <v>16.87</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
@@ -1432,33 +1360,33 @@
         <v>3</v>
       </c>
       <c r="L25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" t="n">
-        <v>19.2</v>
+        <v>15.2</v>
       </c>
       <c r="C26" t="n">
         <v>8</v>
       </c>
       <c r="D26" t="n">
-        <v>400</v>
+        <v>304</v>
       </c>
       <c r="E26" t="n">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="F26" t="n">
-        <v>3.08</v>
+        <v>3.15</v>
       </c>
       <c r="G26" t="n">
-        <v>3.845</v>
+        <v>3.435</v>
       </c>
       <c r="H26" t="n">
-        <v>17.05</v>
+        <v>17.3</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -1475,75 +1403,75 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" t="n">
-        <v>27.3</v>
+        <v>13.3</v>
       </c>
       <c r="C27" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D27" t="n">
-        <v>79</v>
+        <v>350</v>
       </c>
       <c r="E27" t="n">
-        <v>66</v>
+        <v>245</v>
       </c>
       <c r="F27" t="n">
-        <v>4.08</v>
+        <v>3.73</v>
       </c>
       <c r="G27" t="n">
-        <v>1.935</v>
+        <v>3.84</v>
       </c>
       <c r="H27" t="n">
-        <v>18.9</v>
+        <v>15.41</v>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L27" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" t="n">
-        <v>26</v>
+        <v>19.2</v>
       </c>
       <c r="C28" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D28" t="n">
-        <v>120.3</v>
+        <v>400</v>
       </c>
       <c r="E28" t="n">
-        <v>91</v>
+        <v>175</v>
       </c>
       <c r="F28" t="n">
-        <v>4.43</v>
+        <v>3.08</v>
       </c>
       <c r="G28" t="n">
-        <v>2.14</v>
+        <v>3.845</v>
       </c>
       <c r="H28" t="n">
-        <v>16.7</v>
+        <v>17.05</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L28" t="n">
         <v>2</v>
@@ -1551,28 +1479,28 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" t="n">
-        <v>30.4</v>
+        <v>27.3</v>
       </c>
       <c r="C29" t="n">
         <v>4</v>
       </c>
       <c r="D29" t="n">
-        <v>95.1</v>
+        <v>79</v>
       </c>
       <c r="E29" t="n">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="F29" t="n">
-        <v>3.77</v>
+        <v>4.08</v>
       </c>
       <c r="G29" t="n">
-        <v>1.513</v>
+        <v>1.935</v>
       </c>
       <c r="H29" t="n">
-        <v>16.9</v>
+        <v>18.9</v>
       </c>
       <c r="I29" t="n">
         <v>1</v>
@@ -1581,36 +1509,36 @@
         <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" t="n">
-        <v>15.8</v>
+        <v>26</v>
       </c>
       <c r="C30" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D30" t="n">
-        <v>351</v>
+        <v>120.3</v>
       </c>
       <c r="E30" t="n">
-        <v>264</v>
+        <v>91</v>
       </c>
       <c r="F30" t="n">
-        <v>4.22</v>
+        <v>4.43</v>
       </c>
       <c r="G30" t="n">
-        <v>3.17</v>
+        <v>2.14</v>
       </c>
       <c r="H30" t="n">
-        <v>14.5</v>
+        <v>16.7</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
@@ -1622,36 +1550,36 @@
         <v>5</v>
       </c>
       <c r="L30" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" t="n">
-        <v>19.7</v>
+        <v>30.4</v>
       </c>
       <c r="C31" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D31" t="n">
-        <v>145</v>
+        <v>95.1</v>
       </c>
       <c r="E31" t="n">
-        <v>175</v>
+        <v>113</v>
       </c>
       <c r="F31" t="n">
-        <v>3.62</v>
+        <v>3.77</v>
       </c>
       <c r="G31" t="n">
-        <v>2.77</v>
+        <v>1.513</v>
       </c>
       <c r="H31" t="n">
-        <v>15.5</v>
+        <v>16.9</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="n">
         <v>1</v>
@@ -1660,33 +1588,33 @@
         <v>5</v>
       </c>
       <c r="L31" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32" t="n">
-        <v>15</v>
+        <v>15.8</v>
       </c>
       <c r="C32" t="n">
         <v>8</v>
       </c>
       <c r="D32" t="n">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="E32" t="n">
-        <v>335</v>
+        <v>264</v>
       </c>
       <c r="F32" t="n">
-        <v>3.54</v>
+        <v>4.22</v>
       </c>
       <c r="G32" t="n">
-        <v>3.57</v>
+        <v>3.17</v>
       </c>
       <c r="H32" t="n">
-        <v>14.6</v>
+        <v>14.5</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
@@ -1698,55 +1626,121 @@
         <v>5</v>
       </c>
       <c r="L32" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="n">
+        <v>19.7</v>
+      </c>
+      <c r="C33" t="n">
+        <v>6</v>
+      </c>
+      <c r="D33" t="n">
+        <v>145</v>
+      </c>
+      <c r="E33" t="n">
+        <v>175</v>
+      </c>
+      <c r="F33" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2.77</v>
+      </c>
+      <c r="H33" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" t="n">
+        <v>5</v>
+      </c>
+      <c r="L33" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
         <v>43</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B34" t="n">
+        <v>15</v>
+      </c>
+      <c r="C34" t="n">
+        <v>8</v>
+      </c>
+      <c r="D34" t="n">
+        <v>301</v>
+      </c>
+      <c r="E34" t="n">
+        <v>335</v>
+      </c>
+      <c r="F34" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="H34" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>1</v>
+      </c>
+      <c r="K34" t="n">
+        <v>5</v>
+      </c>
+      <c r="L34" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="n">
         <v>21.4</v>
       </c>
-      <c r="C33" t="n">
-        <v>4</v>
-      </c>
-      <c r="D33" t="n">
+      <c r="C35" t="n">
+        <v>4</v>
+      </c>
+      <c r="D35" t="n">
         <v>121</v>
       </c>
-      <c r="E33" t="n">
+      <c r="E35" t="n">
         <v>109</v>
       </c>
-      <c r="F33" t="n">
+      <c r="F35" t="n">
         <v>4.11</v>
       </c>
-      <c r="G33" t="n">
+      <c r="G35" t="n">
         <v>2.78</v>
       </c>
-      <c r="H33" t="n">
+      <c r="H35" t="n">
         <v>18.6</v>
       </c>
-      <c r="I33" t="n">
-        <v>1</v>
-      </c>
-      <c r="J33" t="n">
-        <v>1</v>
-      </c>
-      <c r="K33" t="n">
-        <v>4</v>
-      </c>
-      <c r="L33" t="n">
+      <c r="I35" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" t="n">
+        <v>1</v>
+      </c>
+      <c r="K35" t="n">
+        <v>4</v>
+      </c>
+      <c r="L35" t="n">
         <v>2</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>